<commit_message>
- changed:  Projektkennzahlen aktualisiert - added: Statusbericht 6 (19.08.)
</commit_message>
<xml_diff>
--- a/documents/projectmanagement/2_Definition/Projektkennzahlen.xlsx
+++ b/documents/projectmanagement/2_Definition/Projektkennzahlen.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\PM\documents\projectmanagement\2_Definition\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20460" windowHeight="7680"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -170,17 +165,7 @@
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -469,7 +454,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -479,8 +464,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -593,7 +578,7 @@
         <v>894.44</v>
       </c>
       <c r="G4" s="4">
-        <f t="shared" ref="G4:G7" si="1">E4+F4</f>
+        <f t="shared" ref="G4:G8" si="1">E4+F4</f>
         <v>2029.24</v>
       </c>
       <c r="I4" s="4">
@@ -723,14 +708,26 @@
         <f>1248.94+(2579.69/5)</f>
         <v>1764.8780000000002</v>
       </c>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
+      <c r="B8" s="4">
+        <v>1169.44</v>
+      </c>
+      <c r="C8" s="4">
+        <f>A8+B8</f>
+        <v>2934.3180000000002</v>
+      </c>
+      <c r="E8" s="4">
+        <v>1443.92</v>
+      </c>
+      <c r="F8" s="4">
+        <v>1169.44</v>
+      </c>
+      <c r="G8" s="4">
+        <f t="shared" si="1"/>
+        <v>2613.36</v>
+      </c>
       <c r="I8" s="4">
         <f t="shared" si="2"/>
-        <v>1764.8780000000002</v>
+        <v>320.95800000000008</v>
       </c>
       <c r="J8" s="4">
         <f t="shared" si="0"/>
@@ -738,7 +735,7 @@
       </c>
       <c r="K8" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>320.95800000000008</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
@@ -818,13 +815,13 @@
       <c r="B12" s="4"/>
       <c r="C12" s="4">
         <f>SUM(C3:C11)</f>
-        <v>11782.838</v>
+        <v>14717.155999999999</v>
       </c>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
       <c r="G12" s="4">
         <f>SUM(G3:G11)</f>
-        <v>12383.400000000001</v>
+        <v>14996.760000000002</v>
       </c>
       <c r="I12" s="4">
         <f t="shared" si="2"/>
@@ -836,7 +833,7 @@
       </c>
       <c r="K12" s="4">
         <f>SUM(K3:K11)</f>
-        <v>-600.56200000000013</v>
+        <v>-279.60400000000004</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
@@ -1026,13 +1023,15 @@
       <c r="B22" s="2">
         <v>6</v>
       </c>
-      <c r="E22" s="2"/>
+      <c r="E22" s="2">
+        <v>65</v>
+      </c>
       <c r="F22" s="2">
         <v>6</v>
       </c>
       <c r="I22" s="2">
         <f t="shared" si="4"/>
-        <v>-65</v>
+        <v>0</v>
       </c>
       <c r="J22" s="2">
         <v>6</v>
@@ -1103,10 +1102,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="I3:K12">
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
- modified Projektkennzahlen - modified 6. Projektstatusbericht - added 7. Projektstatusbericht
</commit_message>
<xml_diff>
--- a/documents/projectmanagement/2_Definition/Projektkennzahlen.xlsx
+++ b/documents/projectmanagement/2_Definition/Projektkennzahlen.xlsx
@@ -1,15 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\PM\documents\projectmanagement\2_Definition\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20460" windowHeight="7680"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -454,7 +459,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -465,7 +470,7 @@
   <dimension ref="A1:M25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -534,7 +539,7 @@
         <v>894.44</v>
       </c>
       <c r="C3" s="4">
-        <f>A3+B3</f>
+        <f t="shared" ref="C3:C9" si="0">A3+B3</f>
         <v>2143.38</v>
       </c>
       <c r="E3" s="4">
@@ -552,11 +557,11 @@
         <v>-474.26</v>
       </c>
       <c r="J3" s="4">
-        <f t="shared" ref="J3:K12" si="0">B3-F3</f>
+        <f t="shared" ref="J3:K12" si="1">B3-F3</f>
         <v>0</v>
       </c>
       <c r="K3" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-474.26000000000022</v>
       </c>
     </row>
@@ -568,7 +573,7 @@
         <v>894.44</v>
       </c>
       <c r="C4" s="4">
-        <f>A4+B4</f>
+        <f t="shared" si="0"/>
         <v>2143.38</v>
       </c>
       <c r="E4" s="3">
@@ -578,19 +583,19 @@
         <v>894.44</v>
       </c>
       <c r="G4" s="4">
-        <f t="shared" ref="G4:G8" si="1">E4+F4</f>
+        <f t="shared" ref="G4:G9" si="2">E4+F4</f>
         <v>2029.24</v>
       </c>
       <c r="I4" s="4">
-        <f t="shared" ref="I4:I12" si="2">A4-E4</f>
+        <f t="shared" ref="I4:I12" si="3">A4-E4</f>
         <v>114.1400000000001</v>
       </c>
       <c r="J4" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K4" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>114.1400000000001</v>
       </c>
     </row>
@@ -602,7 +607,7 @@
         <v>894.44</v>
       </c>
       <c r="C5" s="4">
-        <f>A5+B5</f>
+        <f t="shared" si="0"/>
         <v>2143.38</v>
       </c>
       <c r="E5" s="4">
@@ -612,19 +617,19 @@
         <v>894.44</v>
       </c>
       <c r="G5" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2918.6400000000003</v>
       </c>
       <c r="I5" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-775.26</v>
       </c>
       <c r="J5" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K5" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-775.26000000000022</v>
       </c>
     </row>
@@ -636,7 +641,7 @@
         <v>1169.44</v>
       </c>
       <c r="C6" s="4">
-        <f>A6+B6</f>
+        <f t="shared" si="0"/>
         <v>2418.38</v>
       </c>
       <c r="D6" t="s">
@@ -649,19 +654,19 @@
         <v>1169.44</v>
       </c>
       <c r="G6" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2457.84</v>
       </c>
       <c r="I6" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-39.460000000000036</v>
       </c>
       <c r="J6" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K6" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-39.460000000000036</v>
       </c>
     </row>
@@ -674,7 +679,7 @@
         <v>1169.44</v>
       </c>
       <c r="C7" s="4">
-        <f>A7+B7</f>
+        <f t="shared" si="0"/>
         <v>2934.3180000000002</v>
       </c>
       <c r="D7" t="s">
@@ -687,83 +692,93 @@
         <v>1169.44</v>
       </c>
       <c r="G7" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2360.04</v>
       </c>
       <c r="I7" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>574.27800000000025</v>
       </c>
       <c r="J7" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K7" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>574.27800000000025</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
-        <f>1248.94+(2579.69/5)</f>
-        <v>1764.8780000000002</v>
+        <v>3025.51</v>
       </c>
       <c r="B8" s="4">
-        <v>1169.44</v>
+        <v>2004.75</v>
       </c>
       <c r="C8" s="4">
-        <f>A8+B8</f>
-        <v>2934.3180000000002</v>
+        <f t="shared" si="0"/>
+        <v>5030.26</v>
       </c>
       <c r="E8" s="4">
-        <v>1443.92</v>
+        <v>2711.34</v>
       </c>
       <c r="F8" s="4">
-        <v>1169.44</v>
+        <v>2004.75</v>
       </c>
       <c r="G8" s="4">
-        <f t="shared" si="1"/>
-        <v>2613.36</v>
+        <f t="shared" si="2"/>
+        <v>4716.09</v>
       </c>
       <c r="I8" s="4">
-        <f t="shared" si="2"/>
-        <v>320.95800000000008</v>
+        <f t="shared" si="3"/>
+        <v>314.17000000000007</v>
       </c>
       <c r="J8" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K8" s="4">
-        <f t="shared" si="0"/>
-        <v>320.95800000000008</v>
+        <f t="shared" si="1"/>
+        <v>314.17000000000007</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
-        <f t="shared" ref="A9:A11" si="3">1248.94+(2579.69/5)</f>
-        <v>1764.8780000000002</v>
-      </c>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
+        <v>504.25</v>
+      </c>
+      <c r="B9" s="4">
+        <v>334.13</v>
+      </c>
+      <c r="C9" s="4">
+        <f t="shared" si="0"/>
+        <v>838.38</v>
+      </c>
+      <c r="E9" s="4">
+        <v>490.55</v>
+      </c>
+      <c r="F9" s="4">
+        <v>334.13</v>
+      </c>
+      <c r="G9" s="4">
+        <f t="shared" si="2"/>
+        <v>824.68000000000006</v>
+      </c>
       <c r="I9" s="4">
-        <f t="shared" si="2"/>
-        <v>1764.8780000000002</v>
+        <f t="shared" si="3"/>
+        <v>13.699999999999989</v>
       </c>
       <c r="J9" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K9" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>13.699999999999932</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="A9:A11" si="4">1248.94+(2579.69/5)</f>
         <v>1764.8780000000002</v>
       </c>
       <c r="B10" s="4"/>
@@ -772,21 +787,21 @@
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
       <c r="I10" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1764.8780000000002</v>
       </c>
       <c r="J10" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K10" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1764.8780000000002</v>
       </c>
       <c r="B11" s="4"/>
@@ -795,45 +810,45 @@
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
       <c r="I11" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1764.8780000000002</v>
       </c>
       <c r="J11" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K11" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <f>SUM(A3:A11)</f>
-        <v>13820.150000000003</v>
+        <v>13820.154000000002</v>
       </c>
       <c r="B12" s="4"/>
       <c r="C12" s="4">
         <f>SUM(C3:C11)</f>
-        <v>14717.155999999999</v>
+        <v>17651.477999999999</v>
       </c>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
       <c r="G12" s="4">
         <f>SUM(G3:G11)</f>
-        <v>14996.760000000002</v>
+        <v>17924.170000000002</v>
       </c>
       <c r="I12" s="4">
-        <f t="shared" si="2"/>
-        <v>13820.150000000003</v>
+        <f t="shared" si="3"/>
+        <v>13820.154000000002</v>
       </c>
       <c r="J12" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K12" s="4">
         <f>SUM(K3:K11)</f>
-        <v>-279.60400000000004</v>
+        <v>-272.69200000000012</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
@@ -922,7 +937,7 @@
         <v>2</v>
       </c>
       <c r="I18" s="2">
-        <f t="shared" ref="I18:I25" si="4">E18-A18</f>
+        <f t="shared" ref="I18:I25" si="5">E18-A18</f>
         <v>5</v>
       </c>
       <c r="J18" s="2">
@@ -949,7 +964,7 @@
         <v>3</v>
       </c>
       <c r="I19" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="J19" s="2">
@@ -976,7 +991,7 @@
         <v>4</v>
       </c>
       <c r="I20" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2.5</v>
       </c>
       <c r="J20" s="2">
@@ -1003,7 +1018,7 @@
         <v>5</v>
       </c>
       <c r="I21" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2.5</v>
       </c>
       <c r="J21" s="2">
@@ -1030,7 +1045,7 @@
         <v>6</v>
       </c>
       <c r="I22" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="J22" s="2">
@@ -1055,7 +1070,7 @@
         <v>7</v>
       </c>
       <c r="I23" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-80</v>
       </c>
       <c r="J23" s="2">
@@ -1074,7 +1089,7 @@
         <v>8</v>
       </c>
       <c r="I24" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-95</v>
       </c>
       <c r="J24" s="2">
@@ -1093,7 +1108,7 @@
         <v>9</v>
       </c>
       <c r="I25" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-100</v>
       </c>
       <c r="J25" s="2">

</xml_diff>

<commit_message>
- added: Letzter Statusbericht - modified: Projektkennzahlen
</commit_message>
<xml_diff>
--- a/documents/projectmanagement/2_Definition/Projektkennzahlen.xlsx
+++ b/documents/projectmanagement/2_Definition/Projektkennzahlen.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\PM\documents\projectmanagement\2_Definition\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20460" windowHeight="7680"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -149,7 +144,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -166,6 +161,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -459,7 +455,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -467,10 +463,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M25"/>
+  <dimension ref="A1:M30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -539,7 +535,7 @@
         <v>894.44</v>
       </c>
       <c r="C3" s="4">
-        <f t="shared" ref="C3:C9" si="0">A3+B3</f>
+        <f t="shared" ref="C3:C11" si="0">A3+B3</f>
         <v>2143.38</v>
       </c>
       <c r="E3" s="4">
@@ -583,7 +579,7 @@
         <v>894.44</v>
       </c>
       <c r="G4" s="4">
-        <f t="shared" ref="G4:G9" si="2">E4+F4</f>
+        <f t="shared" ref="G4:G11" si="2">E4+F4</f>
         <v>2029.24</v>
       </c>
       <c r="I4" s="4">
@@ -778,17 +774,28 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
-        <f t="shared" ref="A9:A11" si="4">1248.94+(2579.69/5)</f>
-        <v>1764.8780000000002</v>
-      </c>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
+        <v>1260.6300000000001</v>
+      </c>
+      <c r="B10" s="4">
+        <v>835.31</v>
+      </c>
+      <c r="C10" s="4">
+        <f t="shared" si="0"/>
+        <v>2095.94</v>
+      </c>
+      <c r="E10" s="4">
+        <v>1007.96</v>
+      </c>
+      <c r="F10" s="4">
+        <v>835.31</v>
+      </c>
+      <c r="G10" s="4">
+        <f t="shared" si="2"/>
+        <v>1843.27</v>
+      </c>
       <c r="I10" s="4">
         <f t="shared" si="3"/>
-        <v>1764.8780000000002</v>
+        <v>252.67000000000007</v>
       </c>
       <c r="J10" s="4">
         <f t="shared" si="1"/>
@@ -796,65 +803,85 @@
       </c>
       <c r="K10" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>252.67000000000007</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
-        <f t="shared" si="4"/>
-        <v>1764.8780000000002</v>
-      </c>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
+        <f>((1248.94+(2579.69/5))/5)*8</f>
+        <v>2823.8048000000003</v>
+      </c>
+      <c r="B11" s="4">
+        <f>B6/5*8</f>
+        <v>1871.104</v>
+      </c>
+      <c r="C11" s="4">
+        <f t="shared" si="0"/>
+        <v>4694.9088000000002</v>
+      </c>
+      <c r="E11" s="4">
+        <v>2708.94</v>
+      </c>
+      <c r="F11" s="4">
+        <v>1871.1</v>
+      </c>
+      <c r="G11" s="4">
+        <f t="shared" si="2"/>
+        <v>4580.04</v>
+      </c>
       <c r="I11" s="4">
         <f t="shared" si="3"/>
-        <v>1764.8780000000002</v>
+        <v>114.86480000000029</v>
       </c>
       <c r="J11" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>4.0000000001327862E-3</v>
       </c>
       <c r="K11" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>114.86880000000019</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <f>SUM(A3:A11)</f>
-        <v>13820.154000000002</v>
-      </c>
-      <c r="B12" s="4"/>
+        <v>14374.832800000002</v>
+      </c>
+      <c r="B12" s="4">
+        <f>SUM(B3:B11)</f>
+        <v>10067.494000000001</v>
+      </c>
       <c r="C12" s="4">
         <f>SUM(C3:C11)</f>
-        <v>17651.477999999999</v>
+        <v>24442.326799999999</v>
       </c>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
       <c r="G12" s="4">
         <f>SUM(G3:G11)</f>
-        <v>17924.170000000002</v>
+        <v>24347.480000000003</v>
       </c>
       <c r="I12" s="4">
         <f t="shared" si="3"/>
-        <v>13820.154000000002</v>
+        <v>14374.832800000002</v>
       </c>
       <c r="J12" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>10067.494000000001</v>
       </c>
       <c r="K12" s="4">
         <f>SUM(K3:K11)</f>
-        <v>-272.69200000000012</v>
+        <v>94.846800000000144</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>7</v>
       </c>
+      <c r="D14" s="8">
+        <f>A11-E11</f>
+        <v>114.86480000000029</v>
+      </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B15" s="5" t="s">
@@ -937,7 +964,7 @@
         <v>2</v>
       </c>
       <c r="I18" s="2">
-        <f t="shared" ref="I18:I25" si="5">E18-A18</f>
+        <f t="shared" ref="I18:I25" si="4">E18-A18</f>
         <v>5</v>
       </c>
       <c r="J18" s="2">
@@ -964,7 +991,7 @@
         <v>3</v>
       </c>
       <c r="I19" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
       <c r="J19" s="2">
@@ -991,7 +1018,7 @@
         <v>4</v>
       </c>
       <c r="I20" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>2.5</v>
       </c>
       <c r="J20" s="2">
@@ -1018,7 +1045,7 @@
         <v>5</v>
       </c>
       <c r="I21" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>2.5</v>
       </c>
       <c r="J21" s="2">
@@ -1045,7 +1072,7 @@
         <v>6</v>
       </c>
       <c r="I22" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="J22" s="2">
@@ -1070,7 +1097,7 @@
         <v>7</v>
       </c>
       <c r="I23" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>-80</v>
       </c>
       <c r="J23" s="2">
@@ -1089,7 +1116,7 @@
         <v>8</v>
       </c>
       <c r="I24" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>-95</v>
       </c>
       <c r="J24" s="2">
@@ -1108,11 +1135,17 @@
         <v>9</v>
       </c>
       <c r="I25" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>-100</v>
       </c>
       <c r="J25" s="2">
         <v>9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E30">
+        <f>22476.38-22571.22</f>
+        <v>-94.840000000000146</v>
       </c>
     </row>
   </sheetData>

</xml_diff>